<commit_message>
various, data updates, 0-5 level
</commit_message>
<xml_diff>
--- a/backend/data/activities.xlsx
+++ b/backend/data/activities.xlsx
@@ -1,15 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asi\Documents\GitHub\eventhorizon\backend\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D2BA060-605F-455D-BB81-C3DB4863C539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1774,8 +1793,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1846,18 +1865,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1895,7 +1922,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1929,6 +1956,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1963,9 +1991,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2138,14 +2167,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="AE28" sqref="AE28"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="50.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="12" width="0" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.9296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="27" width="0" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="15.46484375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:39">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2264,7 +2307,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:39">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2302,19 +2345,19 @@
         <v>174</v>
       </c>
       <c r="M2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N2">
         <v>5</v>
       </c>
       <c r="O2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P2" t="s">
         <v>214</v>
       </c>
       <c r="Q2">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="R2">
         <v>7</v>
@@ -2347,7 +2390,7 @@
         <v>435</v>
       </c>
       <c r="AB2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AC2">
         <v>1</v>
@@ -2380,7 +2423,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="3" spans="1:39">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2418,7 +2461,7 @@
         <v>5</v>
       </c>
       <c r="N3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O3">
         <v>3</v>
@@ -2490,7 +2533,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="4" spans="1:39">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2525,13 +2568,13 @@
         <v>176</v>
       </c>
       <c r="M4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N4">
         <v>5</v>
       </c>
       <c r="O4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P4" t="s">
         <v>216</v>
@@ -2567,7 +2610,7 @@
         <v>435</v>
       </c>
       <c r="AB4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AC4">
         <v>1</v>
@@ -2600,7 +2643,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="5" spans="1:39">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2635,19 +2678,19 @@
         <v>177</v>
       </c>
       <c r="M5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N5">
         <v>5</v>
       </c>
       <c r="O5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P5" t="s">
         <v>217</v>
       </c>
       <c r="Q5">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="S5" t="s">
         <v>254</v>
@@ -2677,7 +2720,7 @@
         <v>435</v>
       </c>
       <c r="AB5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AC5">
         <v>1</v>
@@ -2710,7 +2753,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="6" spans="1:39">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2745,10 +2788,10 @@
         <v>178</v>
       </c>
       <c r="M6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O6">
         <v>4</v>
@@ -2787,7 +2830,7 @@
         <v>435</v>
       </c>
       <c r="AB6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AC6">
         <v>2</v>
@@ -2820,7 +2863,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="7" spans="1:39">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2867,7 +2910,7 @@
         <v>219</v>
       </c>
       <c r="Q7">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="S7" t="s">
         <v>256</v>
@@ -2897,7 +2940,7 @@
         <v>435</v>
       </c>
       <c r="AB7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AC7">
         <v>1</v>
@@ -2930,7 +2973,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="8" spans="1:39">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2968,13 +3011,13 @@
         <v>180</v>
       </c>
       <c r="M8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N8">
         <v>1</v>
       </c>
       <c r="O8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P8" t="s">
         <v>220</v>
@@ -3010,7 +3053,7 @@
         <v>436</v>
       </c>
       <c r="AB8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC8">
         <v>3.5</v>
@@ -3046,7 +3089,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="9" spans="1:39">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3081,7 +3124,7 @@
         <v>181</v>
       </c>
       <c r="M9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N9">
         <v>1</v>
@@ -3156,7 +3199,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="10" spans="1:39">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3194,7 +3237,7 @@
         <v>182</v>
       </c>
       <c r="M10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N10">
         <v>2</v>
@@ -3269,7 +3312,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="11" spans="1:39">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3304,13 +3347,13 @@
         <v>183</v>
       </c>
       <c r="M11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N11">
         <v>2</v>
       </c>
       <c r="O11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P11" t="s">
         <v>223</v>
@@ -3346,7 +3389,7 @@
         <v>436</v>
       </c>
       <c r="AB11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC11">
         <v>3.5</v>
@@ -3379,7 +3422,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="12" spans="1:39">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3414,7 +3457,7 @@
         <v>184</v>
       </c>
       <c r="M12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N12">
         <v>1</v>
@@ -3456,7 +3499,7 @@
         <v>436</v>
       </c>
       <c r="AB12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC12">
         <v>3.5</v>
@@ -3489,7 +3532,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="13" spans="1:39">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3524,10 +3567,10 @@
         <v>185</v>
       </c>
       <c r="M13">
+        <v>2</v>
+      </c>
+      <c r="N13">
         <v>3</v>
-      </c>
-      <c r="N13">
-        <v>1</v>
       </c>
       <c r="O13">
         <v>3</v>
@@ -3599,7 +3642,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="14" spans="1:39">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3634,19 +3677,19 @@
         <v>186</v>
       </c>
       <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14">
         <v>2</v>
       </c>
-      <c r="N14">
-        <v>1</v>
-      </c>
       <c r="O14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P14" t="s">
         <v>226</v>
       </c>
       <c r="Q14">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="S14" t="s">
         <v>254</v>
@@ -3676,7 +3719,7 @@
         <v>436</v>
       </c>
       <c r="AB14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC14">
         <v>3.5</v>
@@ -3709,7 +3752,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="15" spans="1:39">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3747,10 +3790,10 @@
         <v>187</v>
       </c>
       <c r="M15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O15">
         <v>4</v>
@@ -3759,7 +3802,7 @@
         <v>227</v>
       </c>
       <c r="Q15">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="S15" t="s">
         <v>254</v>
@@ -3789,7 +3832,7 @@
         <v>437</v>
       </c>
       <c r="AB15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC15">
         <v>3.5</v>
@@ -3825,7 +3868,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="16" spans="1:39">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3863,10 +3906,10 @@
         <v>188</v>
       </c>
       <c r="M16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O16">
         <v>4</v>
@@ -3905,7 +3948,7 @@
         <v>437</v>
       </c>
       <c r="AB16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC16">
         <v>3.5</v>
@@ -3941,7 +3984,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="17" spans="1:39">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3979,10 +4022,10 @@
         <v>189</v>
       </c>
       <c r="M17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O17">
         <v>4</v>
@@ -3991,7 +4034,7 @@
         <v>229</v>
       </c>
       <c r="Q17">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="S17" t="s">
         <v>254</v>
@@ -4021,7 +4064,7 @@
         <v>437</v>
       </c>
       <c r="AB17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC17">
         <v>3.5</v>
@@ -4057,7 +4100,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="18" spans="1:39">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4095,10 +4138,10 @@
         <v>190</v>
       </c>
       <c r="M18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O18">
         <v>4</v>
@@ -4107,7 +4150,7 @@
         <v>230</v>
       </c>
       <c r="Q18">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="S18" t="s">
         <v>254</v>
@@ -4137,7 +4180,7 @@
         <v>437</v>
       </c>
       <c r="AB18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC18">
         <v>3.5</v>
@@ -4173,7 +4216,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="19" spans="1:39">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4211,10 +4254,10 @@
         <v>191</v>
       </c>
       <c r="M19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O19">
         <v>4</v>
@@ -4253,7 +4296,7 @@
         <v>437</v>
       </c>
       <c r="AB19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC19">
         <v>3.5</v>
@@ -4289,7 +4332,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="20" spans="1:39">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4399,7 +4442,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="21" spans="1:39">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4434,13 +4477,13 @@
         <v>193</v>
       </c>
       <c r="M21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P21" t="s">
         <v>233</v>
@@ -4476,7 +4519,7 @@
         <v>436</v>
       </c>
       <c r="AB21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC21">
         <v>3.5</v>
@@ -4509,7 +4552,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="22" spans="1:39">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4544,10 +4587,10 @@
         <v>194</v>
       </c>
       <c r="M22">
+        <v>1</v>
+      </c>
+      <c r="N22">
         <v>2</v>
-      </c>
-      <c r="N22">
-        <v>1</v>
       </c>
       <c r="O22">
         <v>4</v>
@@ -4586,7 +4629,7 @@
         <v>436</v>
       </c>
       <c r="AB22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC22">
         <v>3.5</v>
@@ -4619,7 +4662,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="23" spans="1:39">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4657,10 +4700,10 @@
         <v>195</v>
       </c>
       <c r="M23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O23">
         <v>4</v>
@@ -4699,7 +4742,7 @@
         <v>437</v>
       </c>
       <c r="AB23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC23">
         <v>3.5</v>
@@ -4735,7 +4778,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="24" spans="1:39">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4773,10 +4816,10 @@
         <v>196</v>
       </c>
       <c r="M24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O24">
         <v>4</v>
@@ -4785,7 +4828,7 @@
         <v>236</v>
       </c>
       <c r="Q24">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="S24" t="s">
         <v>254</v>
@@ -4815,7 +4858,7 @@
         <v>437</v>
       </c>
       <c r="AB24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC24">
         <v>3.5</v>
@@ -4851,7 +4894,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="25" spans="1:39">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>24</v>
       </c>
@@ -4889,10 +4932,10 @@
         <v>197</v>
       </c>
       <c r="M25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O25">
         <v>4</v>
@@ -4931,7 +4974,7 @@
         <v>437</v>
       </c>
       <c r="AB25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC25">
         <v>3.5</v>
@@ -4967,7 +5010,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="26" spans="1:39">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>25</v>
       </c>
@@ -5005,10 +5048,10 @@
         <v>198</v>
       </c>
       <c r="M26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O26">
         <v>4</v>
@@ -5017,7 +5060,7 @@
         <v>238</v>
       </c>
       <c r="Q26">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="S26" t="s">
         <v>254</v>
@@ -5047,7 +5090,7 @@
         <v>437</v>
       </c>
       <c r="AB26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC26">
         <v>3.5</v>
@@ -5083,7 +5126,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="27" spans="1:39">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>26</v>
       </c>
@@ -5121,10 +5164,10 @@
         <v>199</v>
       </c>
       <c r="M27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O27">
         <v>4</v>
@@ -5133,7 +5176,7 @@
         <v>239</v>
       </c>
       <c r="Q27">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="S27" t="s">
         <v>254</v>
@@ -5163,7 +5206,7 @@
         <v>437</v>
       </c>
       <c r="AB27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC27">
         <v>3.5</v>
@@ -5196,7 +5239,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="28" spans="1:39">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>27</v>
       </c>
@@ -5234,10 +5277,10 @@
         <v>200</v>
       </c>
       <c r="M28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O28">
         <v>4</v>
@@ -5276,7 +5319,7 @@
         <v>437</v>
       </c>
       <c r="AB28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC28">
         <v>3.5</v>
@@ -5306,7 +5349,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="29" spans="1:39">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>28</v>
       </c>
@@ -5344,16 +5387,16 @@
         <v>5</v>
       </c>
       <c r="N29">
+        <v>2</v>
+      </c>
+      <c r="O29">
         <v>3</v>
-      </c>
-      <c r="O29">
-        <v>2</v>
       </c>
       <c r="P29" t="s">
         <v>241</v>
       </c>
       <c r="Q29">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="S29" t="s">
         <v>255</v>
@@ -5416,7 +5459,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="30" spans="1:39">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>29</v>
       </c>
@@ -5526,7 +5569,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="31" spans="1:39">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>30</v>
       </c>
@@ -5561,19 +5604,19 @@
         <v>203</v>
       </c>
       <c r="M31">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N31">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O31">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P31" t="s">
         <v>243</v>
       </c>
       <c r="Q31">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="S31" t="s">
         <v>254</v>
@@ -5603,7 +5646,7 @@
         <v>435</v>
       </c>
       <c r="AB31">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AC31">
         <v>3</v>
@@ -5636,7 +5679,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="32" spans="1:39">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>31</v>
       </c>
@@ -5674,10 +5717,10 @@
         <v>204</v>
       </c>
       <c r="M32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O32">
         <v>5</v>
@@ -5686,7 +5729,7 @@
         <v>244</v>
       </c>
       <c r="Q32">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="S32" t="s">
         <v>254</v>
@@ -5716,7 +5759,7 @@
         <v>80</v>
       </c>
       <c r="AB32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC32">
         <v>2.5</v>
@@ -5740,7 +5783,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="33" spans="1:39">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>32</v>
       </c>
@@ -5778,10 +5821,10 @@
         <v>205</v>
       </c>
       <c r="M33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O33">
         <v>5</v>
@@ -5790,7 +5833,7 @@
         <v>245</v>
       </c>
       <c r="Q33">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="S33" t="s">
         <v>254</v>
@@ -5820,7 +5863,7 @@
         <v>80</v>
       </c>
       <c r="AB33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC33">
         <v>2.5</v>
@@ -5847,7 +5890,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="34" spans="1:39">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>33</v>
       </c>
@@ -5882,7 +5925,7 @@
         <v>206</v>
       </c>
       <c r="M34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N34">
         <v>2</v>
@@ -5894,7 +5937,7 @@
         <v>246</v>
       </c>
       <c r="Q34">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="S34" t="s">
         <v>254</v>
@@ -5948,7 +5991,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="35" spans="1:39">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>34</v>
       </c>
@@ -5986,10 +6029,10 @@
         <v>207</v>
       </c>
       <c r="M35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O35">
         <v>5</v>
@@ -6028,7 +6071,7 @@
         <v>80</v>
       </c>
       <c r="AB35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC35">
         <v>2.5</v>
@@ -6055,7 +6098,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="36" spans="1:39">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>35</v>
       </c>
@@ -6090,7 +6133,7 @@
         <v>208</v>
       </c>
       <c r="M36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N36">
         <v>3</v>
@@ -6159,7 +6202,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="37" spans="1:39">
+    <row r="37" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>36</v>
       </c>
@@ -6197,10 +6240,10 @@
         <v>209</v>
       </c>
       <c r="M37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O37">
         <v>5</v>
@@ -6239,7 +6282,7 @@
         <v>80</v>
       </c>
       <c r="AB37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC37">
         <v>2.5</v>
@@ -6269,7 +6312,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="38" spans="1:39">
+    <row r="38" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>37</v>
       </c>
@@ -6307,7 +6350,7 @@
         <v>210</v>
       </c>
       <c r="M38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N38">
         <v>3</v>
@@ -6358,7 +6401,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="39" spans="1:39">
+    <row r="39" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>38</v>
       </c>
@@ -6396,10 +6439,10 @@
         <v>211</v>
       </c>
       <c r="M39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O39">
         <v>5</v>
@@ -6423,7 +6466,7 @@
         <v>436</v>
       </c>
       <c r="AB39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC39">
         <v>2</v>
@@ -6447,7 +6490,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="40" spans="1:39">
+    <row r="40" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>39</v>
       </c>
@@ -6485,10 +6528,10 @@
         <v>212</v>
       </c>
       <c r="M40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O40">
         <v>5</v>
@@ -6512,7 +6555,7 @@
         <v>436</v>
       </c>
       <c r="AB40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC40">
         <v>2</v>
@@ -6536,7 +6579,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="41" spans="1:39">
+    <row r="41" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>40</v>
       </c>
@@ -6574,10 +6617,10 @@
         <v>213</v>
       </c>
       <c r="M41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O41">
         <v>5</v>
@@ -6601,7 +6644,7 @@
         <v>436</v>
       </c>
       <c r="AB41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC41">
         <v>3</v>
@@ -6627,190 +6670,190 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1"/>
-    <hyperlink ref="V2" r:id="rId2"/>
-    <hyperlink ref="AG2" r:id="rId3"/>
-    <hyperlink ref="AH2" r:id="rId4"/>
-    <hyperlink ref="AK2" r:id="rId5"/>
-    <hyperlink ref="I3" r:id="rId6"/>
-    <hyperlink ref="V3" r:id="rId7"/>
-    <hyperlink ref="AG3" r:id="rId8"/>
-    <hyperlink ref="AH3" r:id="rId9"/>
-    <hyperlink ref="AK3" r:id="rId10" location="order"/>
-    <hyperlink ref="I4" r:id="rId11"/>
-    <hyperlink ref="V4" r:id="rId12"/>
-    <hyperlink ref="AG4" r:id="rId13"/>
-    <hyperlink ref="AH4" r:id="rId14"/>
-    <hyperlink ref="AK4" r:id="rId15"/>
-    <hyperlink ref="I5" r:id="rId16"/>
-    <hyperlink ref="V5" r:id="rId17"/>
-    <hyperlink ref="AG5" r:id="rId18"/>
-    <hyperlink ref="AH5" r:id="rId19"/>
-    <hyperlink ref="AK5" r:id="rId20" location="rooms"/>
-    <hyperlink ref="I6" r:id="rId21"/>
-    <hyperlink ref="V6" r:id="rId22"/>
-    <hyperlink ref="AG6" r:id="rId23"/>
-    <hyperlink ref="AH6" r:id="rId24"/>
-    <hyperlink ref="AK6" r:id="rId25"/>
-    <hyperlink ref="I7" r:id="rId26"/>
-    <hyperlink ref="V7" r:id="rId27"/>
-    <hyperlink ref="AG7" r:id="rId28"/>
-    <hyperlink ref="AH7" r:id="rId29"/>
-    <hyperlink ref="AK7" r:id="rId30"/>
-    <hyperlink ref="I8" r:id="rId31"/>
-    <hyperlink ref="V8" r:id="rId32"/>
-    <hyperlink ref="AG8" r:id="rId33"/>
-    <hyperlink ref="AH8" r:id="rId34"/>
-    <hyperlink ref="AK8" r:id="rId35"/>
-    <hyperlink ref="AM8" r:id="rId36"/>
-    <hyperlink ref="I9" r:id="rId37"/>
-    <hyperlink ref="V9" r:id="rId38"/>
-    <hyperlink ref="AG9" r:id="rId39"/>
-    <hyperlink ref="AH9" r:id="rId40"/>
-    <hyperlink ref="AK9" r:id="rId41"/>
-    <hyperlink ref="I10" r:id="rId42"/>
-    <hyperlink ref="V10" r:id="rId43"/>
-    <hyperlink ref="AG10" r:id="rId44"/>
-    <hyperlink ref="AH10" r:id="rId45"/>
-    <hyperlink ref="AK10" r:id="rId46"/>
-    <hyperlink ref="I11" r:id="rId47"/>
-    <hyperlink ref="V11" r:id="rId48"/>
-    <hyperlink ref="AG11" r:id="rId49"/>
-    <hyperlink ref="AH11" r:id="rId50"/>
-    <hyperlink ref="AK11" r:id="rId51"/>
-    <hyperlink ref="I12" r:id="rId52"/>
-    <hyperlink ref="V12" r:id="rId53"/>
-    <hyperlink ref="AG12" r:id="rId54"/>
-    <hyperlink ref="AH12" r:id="rId55"/>
-    <hyperlink ref="AK12" r:id="rId56"/>
-    <hyperlink ref="I13" r:id="rId57"/>
-    <hyperlink ref="V13" r:id="rId58"/>
-    <hyperlink ref="AG13" r:id="rId59"/>
-    <hyperlink ref="AH13" r:id="rId60"/>
-    <hyperlink ref="AK13" r:id="rId61"/>
-    <hyperlink ref="I14" r:id="rId62"/>
-    <hyperlink ref="V14" r:id="rId63"/>
-    <hyperlink ref="AG14" r:id="rId64"/>
-    <hyperlink ref="AH14" r:id="rId65"/>
-    <hyperlink ref="AK14" r:id="rId66"/>
-    <hyperlink ref="I15" r:id="rId67"/>
-    <hyperlink ref="V15" r:id="rId68"/>
-    <hyperlink ref="AG15" r:id="rId69"/>
-    <hyperlink ref="AH15" r:id="rId70"/>
-    <hyperlink ref="AK15" r:id="rId71"/>
-    <hyperlink ref="AM15" r:id="rId72"/>
-    <hyperlink ref="I16" r:id="rId73"/>
-    <hyperlink ref="V16" r:id="rId74"/>
-    <hyperlink ref="AG16" r:id="rId75"/>
-    <hyperlink ref="AH16" r:id="rId76"/>
-    <hyperlink ref="AK16" r:id="rId77"/>
-    <hyperlink ref="AM16" r:id="rId78"/>
-    <hyperlink ref="I17" r:id="rId79"/>
-    <hyperlink ref="V17" r:id="rId80"/>
-    <hyperlink ref="AG17" r:id="rId81"/>
-    <hyperlink ref="AH17" r:id="rId82"/>
-    <hyperlink ref="AK17" r:id="rId83"/>
-    <hyperlink ref="AM17" r:id="rId84"/>
-    <hyperlink ref="I18" r:id="rId85"/>
-    <hyperlink ref="V18" r:id="rId86"/>
-    <hyperlink ref="AG18" r:id="rId87"/>
-    <hyperlink ref="AH18" r:id="rId88"/>
-    <hyperlink ref="AK18" r:id="rId89"/>
-    <hyperlink ref="AM18" r:id="rId90"/>
-    <hyperlink ref="I19" r:id="rId91"/>
-    <hyperlink ref="V19" r:id="rId92"/>
-    <hyperlink ref="AG19" r:id="rId93"/>
-    <hyperlink ref="AH19" r:id="rId94"/>
-    <hyperlink ref="AK19" r:id="rId95"/>
-    <hyperlink ref="AM19" r:id="rId96"/>
-    <hyperlink ref="I20" r:id="rId97"/>
-    <hyperlink ref="V20" r:id="rId98"/>
-    <hyperlink ref="AG20" r:id="rId99"/>
-    <hyperlink ref="AH20" r:id="rId100"/>
-    <hyperlink ref="AK20" r:id="rId101"/>
-    <hyperlink ref="I21" r:id="rId102"/>
-    <hyperlink ref="V21" r:id="rId103"/>
-    <hyperlink ref="AG21" r:id="rId104"/>
-    <hyperlink ref="AH21" r:id="rId105"/>
-    <hyperlink ref="AK21" r:id="rId106"/>
-    <hyperlink ref="I22" r:id="rId107"/>
-    <hyperlink ref="V22" r:id="rId108"/>
-    <hyperlink ref="AG22" r:id="rId109"/>
-    <hyperlink ref="AH22" r:id="rId110"/>
-    <hyperlink ref="AK22" r:id="rId111" location="events"/>
-    <hyperlink ref="I23" r:id="rId112"/>
-    <hyperlink ref="V23" r:id="rId113"/>
-    <hyperlink ref="AG23" r:id="rId114"/>
-    <hyperlink ref="AH23" r:id="rId115"/>
-    <hyperlink ref="AK23" r:id="rId116" location="contactform"/>
-    <hyperlink ref="AM23" r:id="rId117" location="speisekarten"/>
-    <hyperlink ref="I24" r:id="rId118"/>
-    <hyperlink ref="V24" r:id="rId119"/>
-    <hyperlink ref="AG24" r:id="rId120"/>
-    <hyperlink ref="AH24" r:id="rId121"/>
-    <hyperlink ref="AK24" r:id="rId122"/>
-    <hyperlink ref="AM24" r:id="rId123"/>
-    <hyperlink ref="I25" r:id="rId124"/>
-    <hyperlink ref="V25" r:id="rId125"/>
-    <hyperlink ref="AG25" r:id="rId126"/>
-    <hyperlink ref="AH25" r:id="rId127"/>
-    <hyperlink ref="AK25" r:id="rId128"/>
-    <hyperlink ref="AM25" r:id="rId129"/>
-    <hyperlink ref="I26" r:id="rId130"/>
-    <hyperlink ref="V26" r:id="rId131"/>
-    <hyperlink ref="AG26" r:id="rId132"/>
-    <hyperlink ref="AH26" r:id="rId133"/>
-    <hyperlink ref="AK26" r:id="rId134"/>
-    <hyperlink ref="AM26" r:id="rId135"/>
-    <hyperlink ref="I27" r:id="rId136"/>
-    <hyperlink ref="V27" r:id="rId137"/>
-    <hyperlink ref="AG27" r:id="rId138"/>
-    <hyperlink ref="AK27" r:id="rId139"/>
-    <hyperlink ref="AM27" r:id="rId140"/>
-    <hyperlink ref="I28" r:id="rId141"/>
-    <hyperlink ref="V28" r:id="rId142"/>
-    <hyperlink ref="AK28" r:id="rId143"/>
-    <hyperlink ref="AM28" r:id="rId144"/>
-    <hyperlink ref="I29" r:id="rId145"/>
-    <hyperlink ref="V29" r:id="rId146"/>
-    <hyperlink ref="AG29" r:id="rId147"/>
-    <hyperlink ref="AH29" r:id="rId148"/>
-    <hyperlink ref="AK29" r:id="rId149"/>
-    <hyperlink ref="I30" r:id="rId150"/>
-    <hyperlink ref="V30" r:id="rId151"/>
-    <hyperlink ref="AG30" r:id="rId152"/>
-    <hyperlink ref="AH30" r:id="rId153"/>
-    <hyperlink ref="AK30" r:id="rId154"/>
-    <hyperlink ref="I31" r:id="rId155"/>
-    <hyperlink ref="V31" r:id="rId156"/>
-    <hyperlink ref="AG31" r:id="rId157"/>
-    <hyperlink ref="AH31" r:id="rId158"/>
-    <hyperlink ref="AK31" r:id="rId159"/>
-    <hyperlink ref="I32" r:id="rId160"/>
-    <hyperlink ref="V32" r:id="rId161"/>
-    <hyperlink ref="I33" r:id="rId162"/>
-    <hyperlink ref="V33" r:id="rId163"/>
-    <hyperlink ref="AK33" r:id="rId164"/>
-    <hyperlink ref="AM33" r:id="rId165"/>
-    <hyperlink ref="I34" r:id="rId166"/>
-    <hyperlink ref="V34" r:id="rId167"/>
-    <hyperlink ref="AK34" r:id="rId168"/>
-    <hyperlink ref="I35" r:id="rId169"/>
-    <hyperlink ref="V35" r:id="rId170"/>
-    <hyperlink ref="AK35" r:id="rId171"/>
-    <hyperlink ref="AM35" r:id="rId172"/>
-    <hyperlink ref="I36" r:id="rId173"/>
-    <hyperlink ref="V36" r:id="rId174"/>
-    <hyperlink ref="AK36" r:id="rId175"/>
-    <hyperlink ref="AM36" r:id="rId176"/>
-    <hyperlink ref="I37" r:id="rId177"/>
-    <hyperlink ref="V37" r:id="rId178"/>
-    <hyperlink ref="AK37" r:id="rId179"/>
-    <hyperlink ref="AM37" r:id="rId180"/>
-    <hyperlink ref="I38" r:id="rId181"/>
-    <hyperlink ref="I39" r:id="rId182"/>
-    <hyperlink ref="I40" r:id="rId183"/>
-    <hyperlink ref="I41" r:id="rId184"/>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="V2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="AG2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="AH2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="AK2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="I3" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="V3" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="AG3" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="AH3" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="AK3" r:id="rId10" location="order" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="I4" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="V4" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="AG4" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="AH4" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="AK4" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="I5" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="V5" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="AG5" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="AH5" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="AK5" r:id="rId20" location="rooms" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="I6" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="V6" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="AG6" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="AH6" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="AK6" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="I7" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="V7" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="AG7" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="AH7" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="AK7" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="I8" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="V8" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="AG8" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="AH8" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="AK8" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="AM8" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="I9" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="V9" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="AG9" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="AH9" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="AK9" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="I10" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="V10" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="AG10" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="AH10" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="AK10" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="I11" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="V11" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="AG11" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="AH11" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="AK11" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="I12" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="V12" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="AG12" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="AH12" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="AK12" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="I13" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="V13" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="AG13" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="AH13" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="AK13" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="I14" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="V14" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="AG14" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="AH14" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="AK14" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="I15" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="V15" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="AG15" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="AH15" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="AK15" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="AM15" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="I16" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="V16" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="AG16" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="AH16" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="AK16" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="AM16" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="I17" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="V17" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="AG17" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="AH17" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="AK17" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="AM17" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="I18" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="V18" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="AG18" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="AH18" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="AK18" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="AM18" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="I19" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="V19" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="AG19" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="AH19" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="AK19" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="AM19" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="I20" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="V20" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="AG20" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="AH20" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="AK20" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="I21" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="V21" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="AG21" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="AH21" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="AK21" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="I22" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="V22" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="AG22" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="AH22" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="AK22" r:id="rId111" location="events" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="I23" r:id="rId112" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="V23" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="AG23" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="AH23" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="AK23" r:id="rId116" location="contactform" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="AM23" r:id="rId117" location="speisekarten" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="I24" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="V24" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="AG24" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="AH24" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="AK24" r:id="rId122" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="AM24" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
+    <hyperlink ref="I25" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="V25" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
+    <hyperlink ref="AG25" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
+    <hyperlink ref="AH25" r:id="rId127" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
+    <hyperlink ref="AK25" r:id="rId128" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="AM25" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
+    <hyperlink ref="I26" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
+    <hyperlink ref="V26" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
+    <hyperlink ref="AG26" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
+    <hyperlink ref="AH26" r:id="rId133" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
+    <hyperlink ref="AK26" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
+    <hyperlink ref="AM26" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
+    <hyperlink ref="I27" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
+    <hyperlink ref="V27" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
+    <hyperlink ref="AG27" r:id="rId138" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
+    <hyperlink ref="AK27" r:id="rId139" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
+    <hyperlink ref="AM27" r:id="rId140" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
+    <hyperlink ref="I28" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
+    <hyperlink ref="V28" r:id="rId142" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
+    <hyperlink ref="AK28" r:id="rId143" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
+    <hyperlink ref="AM28" r:id="rId144" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
+    <hyperlink ref="I29" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
+    <hyperlink ref="V29" r:id="rId146" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
+    <hyperlink ref="AG29" r:id="rId147" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
+    <hyperlink ref="AH29" r:id="rId148" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
+    <hyperlink ref="AK29" r:id="rId149" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
+    <hyperlink ref="I30" r:id="rId150" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
+    <hyperlink ref="V30" r:id="rId151" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
+    <hyperlink ref="AG30" r:id="rId152" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
+    <hyperlink ref="AH30" r:id="rId153" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
+    <hyperlink ref="AK30" r:id="rId154" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
+    <hyperlink ref="I31" r:id="rId155" xr:uid="{00000000-0004-0000-0000-00009A000000}"/>
+    <hyperlink ref="V31" r:id="rId156" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
+    <hyperlink ref="AG31" r:id="rId157" xr:uid="{00000000-0004-0000-0000-00009C000000}"/>
+    <hyperlink ref="AH31" r:id="rId158" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
+    <hyperlink ref="AK31" r:id="rId159" xr:uid="{00000000-0004-0000-0000-00009E000000}"/>
+    <hyperlink ref="I32" r:id="rId160" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
+    <hyperlink ref="V32" r:id="rId161" xr:uid="{00000000-0004-0000-0000-0000A0000000}"/>
+    <hyperlink ref="I33" r:id="rId162" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
+    <hyperlink ref="V33" r:id="rId163" xr:uid="{00000000-0004-0000-0000-0000A2000000}"/>
+    <hyperlink ref="AK33" r:id="rId164" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
+    <hyperlink ref="AM33" r:id="rId165" xr:uid="{00000000-0004-0000-0000-0000A4000000}"/>
+    <hyperlink ref="I34" r:id="rId166" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
+    <hyperlink ref="V34" r:id="rId167" xr:uid="{00000000-0004-0000-0000-0000A6000000}"/>
+    <hyperlink ref="AK34" r:id="rId168" xr:uid="{00000000-0004-0000-0000-0000A7000000}"/>
+    <hyperlink ref="I35" r:id="rId169" xr:uid="{00000000-0004-0000-0000-0000A8000000}"/>
+    <hyperlink ref="V35" r:id="rId170" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
+    <hyperlink ref="AK35" r:id="rId171" xr:uid="{00000000-0004-0000-0000-0000AA000000}"/>
+    <hyperlink ref="AM35" r:id="rId172" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
+    <hyperlink ref="I36" r:id="rId173" xr:uid="{00000000-0004-0000-0000-0000AC000000}"/>
+    <hyperlink ref="V36" r:id="rId174" xr:uid="{00000000-0004-0000-0000-0000AD000000}"/>
+    <hyperlink ref="AK36" r:id="rId175" xr:uid="{00000000-0004-0000-0000-0000AE000000}"/>
+    <hyperlink ref="AM36" r:id="rId176" xr:uid="{00000000-0004-0000-0000-0000AF000000}"/>
+    <hyperlink ref="I37" r:id="rId177" xr:uid="{00000000-0004-0000-0000-0000B0000000}"/>
+    <hyperlink ref="V37" r:id="rId178" xr:uid="{00000000-0004-0000-0000-0000B1000000}"/>
+    <hyperlink ref="AK37" r:id="rId179" xr:uid="{00000000-0004-0000-0000-0000B2000000}"/>
+    <hyperlink ref="AM37" r:id="rId180" xr:uid="{00000000-0004-0000-0000-0000B3000000}"/>
+    <hyperlink ref="I38" r:id="rId181" xr:uid="{00000000-0004-0000-0000-0000B4000000}"/>
+    <hyperlink ref="I39" r:id="rId182" xr:uid="{00000000-0004-0000-0000-0000B5000000}"/>
+    <hyperlink ref="I40" r:id="rId183" xr:uid="{00000000-0004-0000-0000-0000B6000000}"/>
+    <hyperlink ref="I41" r:id="rId184" xr:uid="{00000000-0004-0000-0000-0000B7000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>